<commit_message>
reduce vgpr for 4096
</commit_message>
<xml_diff>
--- a/work_3d_dev/perf counter.xlsx
+++ b/work_3d_dev/perf counter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\source\repos\fft_test\rocfft_3d_dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\source\repos\fft_test\work_3d_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E372B0CB-5EF6-47E4-9B15-8E78F168443E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017757F0-8F38-40D7-BA45-795AB27D1E0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="perf counter" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="lds_wr" sheetId="11" r:id="rId11"/>
     <sheet name="mem stall" sheetId="14" r:id="rId12"/>
     <sheet name="Sheet1" sheetId="16" r:id="rId13"/>
+    <sheet name="Sheet2" sheetId="17" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="169">
   <si>
     <t>fft_fwd_ip_len50</t>
   </si>
@@ -529,6 +530,30 @@
   <si>
     <t>sin</t>
   </si>
+  <si>
+    <t>instr 1</t>
+  </si>
+  <si>
+    <t>instr 0</t>
+  </si>
+  <si>
+    <t>instr 2</t>
+  </si>
+  <si>
+    <t>……</t>
+  </si>
+  <si>
+    <t>memory address (DWORD)</t>
+  </si>
+  <si>
+    <t>thrd 0</t>
+  </si>
+  <si>
+    <t>thrd 1</t>
+  </si>
+  <si>
+    <t>thrd 2</t>
+  </si>
 </sst>
 </file>
 
@@ -557,7 +582,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -684,8 +709,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="65">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -1503,11 +1534,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="326">
+  <cellXfs count="354">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2337,6 +2390,33 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2355,6 +2435,78 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2376,78 +2528,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2457,32 +2537,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2499,6 +2636,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3E1A46B-CE66-4D69-882E-501EFF6543A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2794000" y="838200"/>
+          <a:ext cx="520700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4243,14 +4438,14 @@
       <c r="C3" s="132"/>
       <c r="D3" s="133"/>
       <c r="E3" s="103"/>
-      <c r="F3" s="283" t="s">
+      <c r="F3" s="316" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="284"/>
-      <c r="H3" s="283" t="s">
+      <c r="G3" s="317"/>
+      <c r="H3" s="316" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="284"/>
+      <c r="I3" s="317"/>
       <c r="J3" s="79"/>
       <c r="K3" s="79"/>
       <c r="L3" s="79"/>
@@ -4324,7 +4519,7 @@
       <c r="B5" s="98">
         <v>2</v>
       </c>
-      <c r="C5" s="285" t="s">
+      <c r="C5" s="318" t="s">
         <v>72</v>
       </c>
       <c r="BN5" s="82"/>
@@ -4335,7 +4530,7 @@
       <c r="B6" s="98">
         <v>3</v>
       </c>
-      <c r="C6" s="286"/>
+      <c r="C6" s="319"/>
       <c r="BN6" s="82"/>
       <c r="BO6" s="76"/>
     </row>
@@ -4344,7 +4539,7 @@
       <c r="B7" s="98">
         <v>4</v>
       </c>
-      <c r="C7" s="287"/>
+      <c r="C7" s="320"/>
       <c r="BN7" s="82"/>
       <c r="BO7" s="76"/>
     </row>
@@ -4353,7 +4548,7 @@
       <c r="B8" s="98">
         <v>5</v>
       </c>
-      <c r="C8" s="288" t="s">
+      <c r="C8" s="321" t="s">
         <v>67</v>
       </c>
       <c r="BN8" s="82"/>
@@ -4364,7 +4559,7 @@
       <c r="B9" s="98">
         <v>6</v>
       </c>
-      <c r="C9" s="289"/>
+      <c r="C9" s="322"/>
       <c r="BN9" s="82"/>
       <c r="BO9" s="76"/>
     </row>
@@ -5457,40 +5652,40 @@
     </row>
     <row r="71" spans="1:67" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B71" s="145"/>
-      <c r="C71" s="299" t="s">
+      <c r="C71" s="301" t="s">
         <v>96</v>
       </c>
-      <c r="D71" s="300"/>
-      <c r="E71" s="300"/>
-      <c r="F71" s="300"/>
-      <c r="G71" s="300"/>
-      <c r="H71" s="300"/>
-      <c r="I71" s="300"/>
-      <c r="J71" s="300"/>
-      <c r="K71" s="300"/>
-      <c r="L71" s="300"/>
-      <c r="M71" s="300"/>
-      <c r="N71" s="300"/>
-      <c r="O71" s="300"/>
-      <c r="P71" s="300"/>
-      <c r="Q71" s="300"/>
-      <c r="R71" s="300"/>
-      <c r="S71" s="300"/>
-      <c r="T71" s="300"/>
-      <c r="U71" s="300"/>
-      <c r="V71" s="300"/>
-      <c r="W71" s="300"/>
-      <c r="X71" s="300"/>
-      <c r="Y71" s="300"/>
-      <c r="Z71" s="300"/>
-      <c r="AA71" s="300"/>
-      <c r="AB71" s="300"/>
-      <c r="AC71" s="300"/>
-      <c r="AD71" s="300"/>
-      <c r="AE71" s="300"/>
-      <c r="AF71" s="300"/>
-      <c r="AG71" s="300"/>
-      <c r="AH71" s="301"/>
+      <c r="D71" s="302"/>
+      <c r="E71" s="302"/>
+      <c r="F71" s="302"/>
+      <c r="G71" s="302"/>
+      <c r="H71" s="302"/>
+      <c r="I71" s="302"/>
+      <c r="J71" s="302"/>
+      <c r="K71" s="302"/>
+      <c r="L71" s="302"/>
+      <c r="M71" s="302"/>
+      <c r="N71" s="302"/>
+      <c r="O71" s="302"/>
+      <c r="P71" s="302"/>
+      <c r="Q71" s="302"/>
+      <c r="R71" s="302"/>
+      <c r="S71" s="302"/>
+      <c r="T71" s="302"/>
+      <c r="U71" s="302"/>
+      <c r="V71" s="302"/>
+      <c r="W71" s="302"/>
+      <c r="X71" s="302"/>
+      <c r="Y71" s="302"/>
+      <c r="Z71" s="302"/>
+      <c r="AA71" s="302"/>
+      <c r="AB71" s="302"/>
+      <c r="AC71" s="302"/>
+      <c r="AD71" s="302"/>
+      <c r="AE71" s="302"/>
+      <c r="AF71" s="302"/>
+      <c r="AG71" s="302"/>
+      <c r="AH71" s="303"/>
       <c r="AI71" s="76"/>
     </row>
     <row r="72" spans="1:67" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5498,48 +5693,48 @@
       <c r="C72" s="293" t="s">
         <v>97</v>
       </c>
-      <c r="D72" s="294"/>
-      <c r="E72" s="294"/>
-      <c r="F72" s="294"/>
-      <c r="G72" s="294"/>
-      <c r="H72" s="294"/>
-      <c r="I72" s="294"/>
-      <c r="J72" s="294"/>
+      <c r="D72" s="292"/>
+      <c r="E72" s="292"/>
+      <c r="F72" s="292"/>
+      <c r="G72" s="292"/>
+      <c r="H72" s="292"/>
+      <c r="I72" s="292"/>
+      <c r="J72" s="292"/>
       <c r="K72" s="293" t="s">
         <v>98</v>
       </c>
-      <c r="L72" s="294"/>
-      <c r="M72" s="294"/>
-      <c r="N72" s="294"/>
-      <c r="O72" s="294"/>
-      <c r="P72" s="294"/>
-      <c r="Q72" s="294"/>
-      <c r="R72" s="295"/>
-      <c r="S72" s="296" t="s">
+      <c r="L72" s="292"/>
+      <c r="M72" s="292"/>
+      <c r="N72" s="292"/>
+      <c r="O72" s="292"/>
+      <c r="P72" s="292"/>
+      <c r="Q72" s="292"/>
+      <c r="R72" s="294"/>
+      <c r="S72" s="295" t="s">
         <v>99</v>
       </c>
-      <c r="T72" s="297"/>
-      <c r="U72" s="297"/>
-      <c r="V72" s="297"/>
-      <c r="W72" s="297"/>
-      <c r="X72" s="297"/>
-      <c r="Y72" s="297"/>
-      <c r="Z72" s="297"/>
-      <c r="AA72" s="296" t="s">
+      <c r="T72" s="296"/>
+      <c r="U72" s="296"/>
+      <c r="V72" s="296"/>
+      <c r="W72" s="296"/>
+      <c r="X72" s="296"/>
+      <c r="Y72" s="296"/>
+      <c r="Z72" s="296"/>
+      <c r="AA72" s="295" t="s">
         <v>100</v>
       </c>
-      <c r="AB72" s="297"/>
-      <c r="AC72" s="297"/>
-      <c r="AD72" s="297"/>
-      <c r="AE72" s="297"/>
-      <c r="AF72" s="297"/>
-      <c r="AG72" s="297"/>
-      <c r="AH72" s="298"/>
+      <c r="AB72" s="296"/>
+      <c r="AC72" s="296"/>
+      <c r="AD72" s="296"/>
+      <c r="AE72" s="296"/>
+      <c r="AF72" s="296"/>
+      <c r="AG72" s="296"/>
+      <c r="AH72" s="297"/>
       <c r="AI72" s="76"/>
     </row>
     <row r="73" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A73" s="145"/>
-      <c r="B73" s="290" t="s">
+      <c r="B73" s="314" t="s">
         <v>92</v>
       </c>
       <c r="C73" s="177">
@@ -5642,7 +5837,7 @@
     </row>
     <row r="74" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A74" s="145"/>
-      <c r="B74" s="291"/>
+      <c r="B74" s="313"/>
       <c r="C74" s="170">
         <v>32</v>
       </c>
@@ -5743,7 +5938,7 @@
     </row>
     <row r="75" spans="1:67" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="145"/>
-      <c r="B75" s="292"/>
+      <c r="B75" s="315"/>
       <c r="C75" s="81">
         <v>64</v>
       </c>
@@ -5844,7 +6039,7 @@
     </row>
     <row r="76" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A76" s="145"/>
-      <c r="B76" s="291" t="s">
+      <c r="B76" s="313" t="s">
         <v>93</v>
       </c>
       <c r="C76" s="81">
@@ -5947,7 +6142,7 @@
     </row>
     <row r="77" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A77" s="145"/>
-      <c r="B77" s="291"/>
+      <c r="B77" s="313"/>
       <c r="C77" s="130">
         <v>28</v>
       </c>
@@ -6048,7 +6243,7 @@
     </row>
     <row r="78" spans="1:67" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="145"/>
-      <c r="B78" s="291"/>
+      <c r="B78" s="313"/>
       <c r="C78" s="86">
         <v>60</v>
       </c>
@@ -6149,7 +6344,7 @@
     </row>
     <row r="79" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A79" s="145"/>
-      <c r="B79" s="290" t="s">
+      <c r="B79" s="314" t="s">
         <v>94</v>
       </c>
       <c r="C79" s="81">
@@ -6252,7 +6447,7 @@
     </row>
     <row r="80" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A80" s="145"/>
-      <c r="B80" s="291"/>
+      <c r="B80" s="313"/>
       <c r="C80" s="130">
         <v>24</v>
       </c>
@@ -6353,7 +6548,7 @@
     </row>
     <row r="81" spans="1:75" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="145"/>
-      <c r="B81" s="292"/>
+      <c r="B81" s="315"/>
       <c r="C81" s="86">
         <v>56</v>
       </c>
@@ -6454,7 +6649,7 @@
     </row>
     <row r="82" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A82" s="145"/>
-      <c r="B82" s="291" t="s">
+      <c r="B82" s="313" t="s">
         <v>95</v>
       </c>
       <c r="C82" s="81">
@@ -6557,7 +6752,7 @@
     </row>
     <row r="83" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A83" s="145"/>
-      <c r="B83" s="291"/>
+      <c r="B83" s="313"/>
       <c r="C83" s="130">
         <v>20</v>
       </c>
@@ -6658,7 +6853,7 @@
     </row>
     <row r="84" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A84" s="145"/>
-      <c r="B84" s="291"/>
+      <c r="B84" s="313"/>
       <c r="C84" s="86">
         <v>52</v>
       </c>
@@ -6759,7 +6954,7 @@
     </row>
     <row r="85" spans="1:75" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="145"/>
-      <c r="B85" s="292"/>
+      <c r="B85" s="315"/>
       <c r="C85" s="81">
         <v>84</v>
       </c>
@@ -6808,86 +7003,86 @@
       <c r="R85" s="82">
         <v>99</v>
       </c>
-      <c r="S85" s="302" t="s">
+      <c r="S85" s="304" t="s">
         <v>104</v>
       </c>
-      <c r="T85" s="303"/>
-      <c r="U85" s="303"/>
-      <c r="V85" s="303"/>
-      <c r="W85" s="303"/>
-      <c r="X85" s="303"/>
-      <c r="Y85" s="303"/>
-      <c r="Z85" s="303"/>
-      <c r="AA85" s="303"/>
-      <c r="AB85" s="303"/>
-      <c r="AC85" s="303"/>
-      <c r="AD85" s="303"/>
-      <c r="AE85" s="303"/>
-      <c r="AF85" s="303"/>
-      <c r="AG85" s="303"/>
-      <c r="AH85" s="304"/>
+      <c r="T85" s="305"/>
+      <c r="U85" s="305"/>
+      <c r="V85" s="305"/>
+      <c r="W85" s="305"/>
+      <c r="X85" s="305"/>
+      <c r="Y85" s="305"/>
+      <c r="Z85" s="305"/>
+      <c r="AA85" s="305"/>
+      <c r="AB85" s="305"/>
+      <c r="AC85" s="305"/>
+      <c r="AD85" s="305"/>
+      <c r="AE85" s="305"/>
+      <c r="AF85" s="305"/>
+      <c r="AG85" s="305"/>
+      <c r="AH85" s="306"/>
       <c r="AI85" s="76"/>
     </row>
     <row r="86" spans="1:75" x14ac:dyDescent="0.35">
       <c r="B86" s="174"/>
-      <c r="C86" s="305" t="s">
+      <c r="C86" s="307" t="s">
         <v>101</v>
       </c>
-      <c r="D86" s="306"/>
-      <c r="E86" s="306"/>
-      <c r="F86" s="306"/>
-      <c r="G86" s="306"/>
-      <c r="H86" s="306"/>
-      <c r="I86" s="306"/>
-      <c r="J86" s="306"/>
-      <c r="K86" s="306"/>
-      <c r="L86" s="306"/>
-      <c r="M86" s="306"/>
-      <c r="N86" s="306"/>
-      <c r="O86" s="306"/>
-      <c r="P86" s="306"/>
-      <c r="Q86" s="306"/>
-      <c r="R86" s="307"/>
-      <c r="S86" s="308" t="s">
+      <c r="D86" s="308"/>
+      <c r="E86" s="308"/>
+      <c r="F86" s="308"/>
+      <c r="G86" s="308"/>
+      <c r="H86" s="308"/>
+      <c r="I86" s="308"/>
+      <c r="J86" s="308"/>
+      <c r="K86" s="308"/>
+      <c r="L86" s="308"/>
+      <c r="M86" s="308"/>
+      <c r="N86" s="308"/>
+      <c r="O86" s="308"/>
+      <c r="P86" s="308"/>
+      <c r="Q86" s="308"/>
+      <c r="R86" s="309"/>
+      <c r="S86" s="310" t="s">
         <v>102</v>
       </c>
-      <c r="T86" s="309"/>
-      <c r="U86" s="309"/>
-      <c r="V86" s="309"/>
-      <c r="W86" s="309"/>
-      <c r="X86" s="309"/>
-      <c r="Y86" s="309"/>
-      <c r="Z86" s="309"/>
-      <c r="AA86" s="309"/>
-      <c r="AB86" s="309"/>
-      <c r="AC86" s="309"/>
-      <c r="AD86" s="309"/>
-      <c r="AE86" s="309"/>
-      <c r="AF86" s="309"/>
-      <c r="AG86" s="309"/>
-      <c r="AH86" s="310"/>
+      <c r="T86" s="311"/>
+      <c r="U86" s="311"/>
+      <c r="V86" s="311"/>
+      <c r="W86" s="311"/>
+      <c r="X86" s="311"/>
+      <c r="Y86" s="311"/>
+      <c r="Z86" s="311"/>
+      <c r="AA86" s="311"/>
+      <c r="AB86" s="311"/>
+      <c r="AC86" s="311"/>
+      <c r="AD86" s="311"/>
+      <c r="AE86" s="311"/>
+      <c r="AF86" s="311"/>
+      <c r="AG86" s="311"/>
+      <c r="AH86" s="312"/>
       <c r="AI86" s="76"/>
     </row>
     <row r="87" spans="1:75" x14ac:dyDescent="0.35">
       <c r="B87" s="145"/>
-      <c r="C87" s="311" t="s">
+      <c r="C87" s="298" t="s">
         <v>103</v>
       </c>
-      <c r="D87" s="312"/>
-      <c r="E87" s="312"/>
-      <c r="F87" s="312"/>
-      <c r="G87" s="312"/>
-      <c r="H87" s="312"/>
-      <c r="I87" s="312"/>
-      <c r="J87" s="312"/>
-      <c r="K87" s="312"/>
-      <c r="L87" s="312"/>
-      <c r="M87" s="312"/>
-      <c r="N87" s="312"/>
-      <c r="O87" s="312"/>
-      <c r="P87" s="312"/>
-      <c r="Q87" s="312"/>
-      <c r="R87" s="313"/>
+      <c r="D87" s="299"/>
+      <c r="E87" s="299"/>
+      <c r="F87" s="299"/>
+      <c r="G87" s="299"/>
+      <c r="H87" s="299"/>
+      <c r="I87" s="299"/>
+      <c r="J87" s="299"/>
+      <c r="K87" s="299"/>
+      <c r="L87" s="299"/>
+      <c r="M87" s="299"/>
+      <c r="N87" s="299"/>
+      <c r="O87" s="299"/>
+      <c r="P87" s="299"/>
+      <c r="Q87" s="299"/>
+      <c r="R87" s="300"/>
       <c r="S87" s="81"/>
       <c r="Z87" s="145"/>
       <c r="AA87" s="81"/>
@@ -7028,102 +7223,102 @@
     </row>
     <row r="92" spans="1:75" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B92" s="145"/>
-      <c r="C92" s="296" t="s">
+      <c r="C92" s="295" t="s">
         <v>105</v>
       </c>
-      <c r="D92" s="297"/>
-      <c r="E92" s="297"/>
-      <c r="F92" s="297"/>
-      <c r="G92" s="296" t="s">
+      <c r="D92" s="296"/>
+      <c r="E92" s="296"/>
+      <c r="F92" s="296"/>
+      <c r="G92" s="295" t="s">
         <v>106</v>
       </c>
-      <c r="H92" s="297"/>
-      <c r="I92" s="297"/>
-      <c r="J92" s="298"/>
-      <c r="K92" s="297" t="s">
+      <c r="H92" s="296"/>
+      <c r="I92" s="296"/>
+      <c r="J92" s="297"/>
+      <c r="K92" s="296" t="s">
         <v>107</v>
       </c>
-      <c r="L92" s="297"/>
-      <c r="M92" s="297"/>
-      <c r="N92" s="297"/>
-      <c r="O92" s="296" t="s">
+      <c r="L92" s="296"/>
+      <c r="M92" s="296"/>
+      <c r="N92" s="296"/>
+      <c r="O92" s="295" t="s">
         <v>108</v>
       </c>
-      <c r="P92" s="297"/>
-      <c r="Q92" s="297"/>
-      <c r="R92" s="298"/>
-      <c r="S92" s="297" t="s">
+      <c r="P92" s="296"/>
+      <c r="Q92" s="296"/>
+      <c r="R92" s="297"/>
+      <c r="S92" s="296" t="s">
         <v>109</v>
       </c>
-      <c r="T92" s="297"/>
-      <c r="U92" s="297"/>
-      <c r="V92" s="297"/>
-      <c r="W92" s="296" t="s">
+      <c r="T92" s="296"/>
+      <c r="U92" s="296"/>
+      <c r="V92" s="296"/>
+      <c r="W92" s="295" t="s">
         <v>110</v>
       </c>
-      <c r="X92" s="297"/>
-      <c r="Y92" s="297"/>
-      <c r="Z92" s="298"/>
-      <c r="AA92" s="297" t="s">
+      <c r="X92" s="296"/>
+      <c r="Y92" s="296"/>
+      <c r="Z92" s="297"/>
+      <c r="AA92" s="296" t="s">
         <v>111</v>
       </c>
-      <c r="AB92" s="297"/>
-      <c r="AC92" s="297"/>
-      <c r="AD92" s="297"/>
-      <c r="AE92" s="296" t="s">
+      <c r="AB92" s="296"/>
+      <c r="AC92" s="296"/>
+      <c r="AD92" s="296"/>
+      <c r="AE92" s="295" t="s">
         <v>112</v>
       </c>
-      <c r="AF92" s="297"/>
-      <c r="AG92" s="297"/>
-      <c r="AH92" s="298"/>
-      <c r="AI92" s="297" t="s">
+      <c r="AF92" s="296"/>
+      <c r="AG92" s="296"/>
+      <c r="AH92" s="297"/>
+      <c r="AI92" s="296" t="s">
         <v>113</v>
       </c>
-      <c r="AJ92" s="297"/>
-      <c r="AK92" s="297"/>
-      <c r="AL92" s="297"/>
-      <c r="AM92" s="296" t="s">
+      <c r="AJ92" s="296"/>
+      <c r="AK92" s="296"/>
+      <c r="AL92" s="296"/>
+      <c r="AM92" s="295" t="s">
         <v>114</v>
       </c>
-      <c r="AN92" s="297"/>
-      <c r="AO92" s="297"/>
-      <c r="AP92" s="298"/>
-      <c r="AQ92" s="297" t="s">
+      <c r="AN92" s="296"/>
+      <c r="AO92" s="296"/>
+      <c r="AP92" s="297"/>
+      <c r="AQ92" s="296" t="s">
         <v>115</v>
       </c>
-      <c r="AR92" s="297"/>
-      <c r="AS92" s="297"/>
-      <c r="AT92" s="297"/>
-      <c r="AU92" s="296" t="s">
+      <c r="AR92" s="296"/>
+      <c r="AS92" s="296"/>
+      <c r="AT92" s="296"/>
+      <c r="AU92" s="295" t="s">
         <v>116</v>
       </c>
-      <c r="AV92" s="297"/>
-      <c r="AW92" s="297"/>
-      <c r="AX92" s="298"/>
-      <c r="AY92" s="294" t="s">
+      <c r="AV92" s="296"/>
+      <c r="AW92" s="296"/>
+      <c r="AX92" s="297"/>
+      <c r="AY92" s="292" t="s">
         <v>117</v>
       </c>
-      <c r="AZ92" s="294"/>
-      <c r="BA92" s="294"/>
-      <c r="BB92" s="294"/>
+      <c r="AZ92" s="292"/>
+      <c r="BA92" s="292"/>
+      <c r="BB92" s="292"/>
       <c r="BC92" s="293" t="s">
         <v>118</v>
       </c>
-      <c r="BD92" s="294"/>
-      <c r="BE92" s="294"/>
-      <c r="BF92" s="295"/>
-      <c r="BG92" s="294" t="s">
+      <c r="BD92" s="292"/>
+      <c r="BE92" s="292"/>
+      <c r="BF92" s="294"/>
+      <c r="BG92" s="292" t="s">
         <v>119</v>
       </c>
-      <c r="BH92" s="294"/>
-      <c r="BI92" s="294"/>
-      <c r="BJ92" s="294"/>
+      <c r="BH92" s="292"/>
+      <c r="BI92" s="292"/>
+      <c r="BJ92" s="292"/>
       <c r="BK92" s="293" t="s">
         <v>120</v>
       </c>
-      <c r="BL92" s="294"/>
-      <c r="BM92" s="294"/>
-      <c r="BN92" s="295"/>
+      <c r="BL92" s="292"/>
+      <c r="BM92" s="292"/>
+      <c r="BN92" s="294"/>
       <c r="BO92" s="76"/>
     </row>
     <row r="93" spans="1:75" x14ac:dyDescent="0.35">
@@ -8280,6 +8475,32 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="C72:J72"/>
+    <mergeCell ref="K72:R72"/>
+    <mergeCell ref="S72:Z72"/>
+    <mergeCell ref="AA72:AH72"/>
+    <mergeCell ref="C71:AH71"/>
+    <mergeCell ref="S85:AH85"/>
+    <mergeCell ref="C86:R86"/>
+    <mergeCell ref="S86:AH86"/>
+    <mergeCell ref="C87:R87"/>
+    <mergeCell ref="C92:F92"/>
+    <mergeCell ref="G92:J92"/>
+    <mergeCell ref="K92:N92"/>
+    <mergeCell ref="O92:R92"/>
+    <mergeCell ref="S92:V92"/>
+    <mergeCell ref="W92:Z92"/>
+    <mergeCell ref="AA92:AD92"/>
+    <mergeCell ref="AE92:AH92"/>
+    <mergeCell ref="AI92:AL92"/>
     <mergeCell ref="BG92:BJ92"/>
     <mergeCell ref="BK92:BN92"/>
     <mergeCell ref="AM92:AP92"/>
@@ -8287,32 +8508,6 @@
     <mergeCell ref="AU92:AX92"/>
     <mergeCell ref="AY92:BB92"/>
     <mergeCell ref="BC92:BF92"/>
-    <mergeCell ref="S92:V92"/>
-    <mergeCell ref="W92:Z92"/>
-    <mergeCell ref="AA92:AD92"/>
-    <mergeCell ref="AE92:AH92"/>
-    <mergeCell ref="AI92:AL92"/>
-    <mergeCell ref="C87:R87"/>
-    <mergeCell ref="C92:F92"/>
-    <mergeCell ref="G92:J92"/>
-    <mergeCell ref="K92:N92"/>
-    <mergeCell ref="O92:R92"/>
-    <mergeCell ref="S72:Z72"/>
-    <mergeCell ref="AA72:AH72"/>
-    <mergeCell ref="C71:AH71"/>
-    <mergeCell ref="S85:AH85"/>
-    <mergeCell ref="C86:R86"/>
-    <mergeCell ref="S86:AH86"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="C72:J72"/>
-    <mergeCell ref="K72:R72"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B73:B75"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8612,14 +8807,14 @@
       </c>
       <c r="C3" s="122"/>
       <c r="D3" s="89"/>
-      <c r="E3" s="314" t="s">
+      <c r="E3" s="323" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="314"/>
-      <c r="G3" s="314" t="s">
+      <c r="F3" s="323"/>
+      <c r="G3" s="323" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="314"/>
+      <c r="H3" s="323"/>
       <c r="I3" s="79"/>
       <c r="J3" s="79"/>
       <c r="K3" s="79"/>
@@ -8727,7 +8922,7 @@
       <c r="B6" s="98">
         <v>3</v>
       </c>
-      <c r="C6" s="315" t="s">
+      <c r="C6" s="324" t="s">
         <v>72</v>
       </c>
       <c r="R6" s="82"/>
@@ -8744,7 +8939,7 @@
       <c r="B7" s="98">
         <v>4</v>
       </c>
-      <c r="C7" s="315"/>
+      <c r="C7" s="324"/>
       <c r="R7" s="82"/>
       <c r="S7" s="81"/>
       <c r="AH7" s="82"/>
@@ -8762,7 +8957,7 @@
       <c r="B8" s="98">
         <v>5</v>
       </c>
-      <c r="C8" s="315"/>
+      <c r="C8" s="324"/>
       <c r="R8" s="82"/>
       <c r="S8" s="81"/>
       <c r="AH8" s="82"/>
@@ -8780,7 +8975,7 @@
       <c r="B9" s="98">
         <v>6</v>
       </c>
-      <c r="C9" s="316" t="s">
+      <c r="C9" s="325" t="s">
         <v>66</v>
       </c>
       <c r="R9" s="82"/>
@@ -8800,7 +8995,7 @@
       <c r="B10" s="98">
         <v>7</v>
       </c>
-      <c r="C10" s="316"/>
+      <c r="C10" s="325"/>
       <c r="R10" s="82"/>
       <c r="S10" s="81"/>
       <c r="AH10" s="82"/>
@@ -9854,7 +10049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65687CC0-31A4-402D-9DD1-AF5B5FD94940}">
   <dimension ref="B3:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -9869,55 +10064,55 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="325" t="s">
+      <c r="B3" s="285" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="325" t="s">
+      <c r="C3" s="285" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="325" t="s">
+      <c r="D3" s="285" t="s">
         <v>153</v>
       </c>
-      <c r="E3" s="325" t="s">
+      <c r="E3" s="285" t="s">
         <v>154</v>
       </c>
-      <c r="F3" s="325" t="s">
+      <c r="F3" s="285" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="325" t="s">
+      <c r="G3" s="285" t="s">
         <v>156</v>
       </c>
-      <c r="H3" s="325" t="s">
+      <c r="H3" s="285" t="s">
         <v>155</v>
       </c>
-      <c r="I3" s="325" t="s">
+      <c r="I3" s="285" t="s">
         <v>157</v>
       </c>
-      <c r="J3" s="325" t="s">
+      <c r="J3" s="285" t="s">
         <v>158</v>
       </c>
-      <c r="K3" s="325" t="s">
+      <c r="K3" s="285" t="s">
         <v>159</v>
       </c>
-      <c r="L3" s="325" t="s">
+      <c r="L3" s="285" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="317">
-        <v>0</v>
-      </c>
-      <c r="C4" s="318">
+      <c r="B4" s="277">
+        <v>0</v>
+      </c>
+      <c r="C4" s="278">
         <f>B4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="318">
-        <v>0</v>
-      </c>
-      <c r="E4" s="318">
-        <v>0</v>
-      </c>
-      <c r="F4" s="319">
+      <c r="D4" s="278">
+        <v>0</v>
+      </c>
+      <c r="E4" s="278">
+        <v>0</v>
+      </c>
+      <c r="F4" s="279">
         <f>9+9*C4+E4</f>
         <v>9</v>
       </c>
@@ -9946,7 +10141,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="320">
+      <c r="B5" s="280">
         <v>1</v>
       </c>
       <c r="C5" s="18">
@@ -9959,7 +10154,7 @@
       <c r="E5" s="18">
         <v>0</v>
       </c>
-      <c r="F5" s="321">
+      <c r="F5" s="281">
         <f t="shared" ref="F5:F33" si="1">9+9*C5+E5</f>
         <v>18</v>
       </c>
@@ -9988,7 +10183,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="320">
+      <c r="B6" s="280">
         <v>2</v>
       </c>
       <c r="C6" s="18">
@@ -10001,7 +10196,7 @@
       <c r="E6" s="18">
         <v>0</v>
       </c>
-      <c r="F6" s="321">
+      <c r="F6" s="281">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
@@ -10030,7 +10225,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="320">
+      <c r="B7" s="280">
         <v>3</v>
       </c>
       <c r="C7" s="18">
@@ -10043,7 +10238,7 @@
       <c r="E7" s="18">
         <v>0</v>
       </c>
-      <c r="F7" s="321">
+      <c r="F7" s="281">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
@@ -10072,7 +10267,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="320">
+      <c r="B8" s="280">
         <v>4</v>
       </c>
       <c r="C8" s="18">
@@ -10085,7 +10280,7 @@
       <c r="E8" s="18">
         <v>0</v>
       </c>
-      <c r="F8" s="321">
+      <c r="F8" s="281">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
@@ -10114,7 +10309,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="320">
+      <c r="B9" s="280">
         <v>5</v>
       </c>
       <c r="C9" s="18">
@@ -10127,7 +10322,7 @@
       <c r="E9" s="18">
         <v>0</v>
       </c>
-      <c r="F9" s="321">
+      <c r="F9" s="281">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
@@ -10156,7 +10351,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="320">
+      <c r="B10" s="280">
         <v>6</v>
       </c>
       <c r="C10" s="18">
@@ -10169,7 +10364,7 @@
       <c r="E10" s="18">
         <v>0</v>
       </c>
-      <c r="F10" s="321">
+      <c r="F10" s="281">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
@@ -10198,7 +10393,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B11" s="320">
+      <c r="B11" s="280">
         <v>7</v>
       </c>
       <c r="C11" s="18">
@@ -10211,7 +10406,7 @@
       <c r="E11" s="18">
         <v>0</v>
       </c>
-      <c r="F11" s="321">
+      <c r="F11" s="281">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
@@ -10240,7 +10435,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="320">
+      <c r="B12" s="280">
         <v>8</v>
       </c>
       <c r="C12" s="18">
@@ -10253,7 +10448,7 @@
       <c r="E12" s="18">
         <v>0</v>
       </c>
-      <c r="F12" s="321">
+      <c r="F12" s="281">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
@@ -10282,20 +10477,20 @@
       </c>
     </row>
     <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="322">
+      <c r="B13" s="282">
         <v>9</v>
       </c>
-      <c r="C13" s="323">
+      <c r="C13" s="283">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D13" s="323">
+      <c r="D13" s="283">
         <v>9</v>
       </c>
-      <c r="E13" s="323">
-        <v>0</v>
-      </c>
-      <c r="F13" s="324">
+      <c r="E13" s="283">
+        <v>0</v>
+      </c>
+      <c r="F13" s="284">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
@@ -10324,20 +10519,20 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="317">
-        <v>0</v>
-      </c>
-      <c r="C14" s="318">
+      <c r="B14" s="277">
+        <v>0</v>
+      </c>
+      <c r="C14" s="278">
         <f>B14</f>
         <v>0</v>
       </c>
-      <c r="D14" s="318">
-        <v>0</v>
-      </c>
-      <c r="E14" s="318">
-        <v>1</v>
-      </c>
-      <c r="F14" s="319">
+      <c r="D14" s="278">
+        <v>0</v>
+      </c>
+      <c r="E14" s="278">
+        <v>1</v>
+      </c>
+      <c r="F14" s="279">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -10366,7 +10561,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="320">
+      <c r="B15" s="280">
         <v>1</v>
       </c>
       <c r="C15" s="18">
@@ -10379,7 +10574,7 @@
       <c r="E15" s="18">
         <v>1</v>
       </c>
-      <c r="F15" s="321">
+      <c r="F15" s="281">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
@@ -10408,7 +10603,7 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="320">
+      <c r="B16" s="280">
         <v>2</v>
       </c>
       <c r="C16" s="18">
@@ -10421,7 +10616,7 @@
       <c r="E16" s="18">
         <v>1</v>
       </c>
-      <c r="F16" s="321">
+      <c r="F16" s="281">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -10450,7 +10645,7 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="320">
+      <c r="B17" s="280">
         <v>3</v>
       </c>
       <c r="C17" s="18">
@@ -10463,7 +10658,7 @@
       <c r="E17" s="18">
         <v>1</v>
       </c>
-      <c r="F17" s="321">
+      <c r="F17" s="281">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
@@ -10492,7 +10687,7 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B18" s="320">
+      <c r="B18" s="280">
         <v>4</v>
       </c>
       <c r="C18" s="18">
@@ -10505,7 +10700,7 @@
       <c r="E18" s="18">
         <v>1</v>
       </c>
-      <c r="F18" s="321">
+      <c r="F18" s="281">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
@@ -10534,7 +10729,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="320">
+      <c r="B19" s="280">
         <v>5</v>
       </c>
       <c r="C19" s="18">
@@ -10547,7 +10742,7 @@
       <c r="E19" s="18">
         <v>1</v>
       </c>
-      <c r="F19" s="321">
+      <c r="F19" s="281">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
@@ -10576,7 +10771,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="320">
+      <c r="B20" s="280">
         <v>6</v>
       </c>
       <c r="C20" s="18">
@@ -10589,7 +10784,7 @@
       <c r="E20" s="18">
         <v>1</v>
       </c>
-      <c r="F20" s="321">
+      <c r="F20" s="281">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
@@ -10618,7 +10813,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="320">
+      <c r="B21" s="280">
         <v>7</v>
       </c>
       <c r="C21" s="18">
@@ -10631,7 +10826,7 @@
       <c r="E21" s="18">
         <v>1</v>
       </c>
-      <c r="F21" s="321">
+      <c r="F21" s="281">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
@@ -10660,7 +10855,7 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="320">
+      <c r="B22" s="280">
         <v>8</v>
       </c>
       <c r="C22" s="18">
@@ -10673,7 +10868,7 @@
       <c r="E22" s="18">
         <v>1</v>
       </c>
-      <c r="F22" s="321">
+      <c r="F22" s="281">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
@@ -10702,20 +10897,20 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="322">
+      <c r="B23" s="282">
         <v>9</v>
       </c>
-      <c r="C23" s="323">
+      <c r="C23" s="283">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D23" s="323">
+      <c r="D23" s="283">
         <v>9</v>
       </c>
-      <c r="E23" s="323">
-        <v>1</v>
-      </c>
-      <c r="F23" s="324">
+      <c r="E23" s="283">
+        <v>1</v>
+      </c>
+      <c r="F23" s="284">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
@@ -10744,20 +10939,20 @@
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="317">
-        <v>0</v>
-      </c>
-      <c r="C24" s="318">
+      <c r="B24" s="277">
+        <v>0</v>
+      </c>
+      <c r="C24" s="278">
         <f>B24</f>
         <v>0</v>
       </c>
-      <c r="D24" s="318">
-        <v>0</v>
-      </c>
-      <c r="E24" s="318">
+      <c r="D24" s="278">
+        <v>0</v>
+      </c>
+      <c r="E24" s="278">
         <v>2</v>
       </c>
-      <c r="F24" s="319">
+      <c r="F24" s="279">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -10786,7 +10981,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="320">
+      <c r="B25" s="280">
         <v>1</v>
       </c>
       <c r="C25" s="18">
@@ -10799,7 +10994,7 @@
       <c r="E25" s="18">
         <v>2</v>
       </c>
-      <c r="F25" s="321">
+      <c r="F25" s="281">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -10828,7 +11023,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="320">
+      <c r="B26" s="280">
         <v>2</v>
       </c>
       <c r="C26" s="18">
@@ -10841,7 +11036,7 @@
       <c r="E26" s="18">
         <v>2</v>
       </c>
-      <c r="F26" s="321">
+      <c r="F26" s="281">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
@@ -10870,7 +11065,7 @@
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="320">
+      <c r="B27" s="280">
         <v>3</v>
       </c>
       <c r="C27" s="18">
@@ -10883,7 +11078,7 @@
       <c r="E27" s="18">
         <v>2</v>
       </c>
-      <c r="F27" s="321">
+      <c r="F27" s="281">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
@@ -10912,7 +11107,7 @@
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="320">
+      <c r="B28" s="280">
         <v>4</v>
       </c>
       <c r="C28" s="18">
@@ -10925,7 +11120,7 @@
       <c r="E28" s="18">
         <v>2</v>
       </c>
-      <c r="F28" s="321">
+      <c r="F28" s="281">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
@@ -10954,7 +11149,7 @@
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="320">
+      <c r="B29" s="280">
         <v>5</v>
       </c>
       <c r="C29" s="18">
@@ -10967,7 +11162,7 @@
       <c r="E29" s="18">
         <v>2</v>
       </c>
-      <c r="F29" s="321">
+      <c r="F29" s="281">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
@@ -10996,7 +11191,7 @@
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B30" s="320">
+      <c r="B30" s="280">
         <v>6</v>
       </c>
       <c r="C30" s="18">
@@ -11009,7 +11204,7 @@
       <c r="E30" s="18">
         <v>2</v>
       </c>
-      <c r="F30" s="321">
+      <c r="F30" s="281">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
@@ -11038,7 +11233,7 @@
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B31" s="320">
+      <c r="B31" s="280">
         <v>7</v>
       </c>
       <c r="C31" s="18">
@@ -11051,7 +11246,7 @@
       <c r="E31" s="18">
         <v>2</v>
       </c>
-      <c r="F31" s="321">
+      <c r="F31" s="281">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
@@ -11080,7 +11275,7 @@
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B32" s="320">
+      <c r="B32" s="280">
         <v>8</v>
       </c>
       <c r="C32" s="18">
@@ -11093,7 +11288,7 @@
       <c r="E32" s="18">
         <v>2</v>
       </c>
-      <c r="F32" s="321">
+      <c r="F32" s="281">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
@@ -11122,20 +11317,20 @@
       </c>
     </row>
     <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="322">
+      <c r="B33" s="282">
         <v>9</v>
       </c>
-      <c r="C33" s="323">
+      <c r="C33" s="283">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D33" s="323">
+      <c r="D33" s="283">
         <v>9</v>
       </c>
-      <c r="E33" s="323">
+      <c r="E33" s="283">
         <v>2</v>
       </c>
-      <c r="F33" s="324">
+      <c r="F33" s="284">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -11165,7 +11360,7 @@
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="I34" s="1">
-        <f t="shared" ref="I5:I34" si="7">H34+1+E34</f>
+        <f t="shared" ref="I34" si="7">H34+1+E34</f>
         <v>1</v>
       </c>
       <c r="K34" s="1">
@@ -11176,6 +11371,247 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D28137B-77C8-470A-8F69-42DBD1097932}">
+  <dimension ref="C5:X13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="35" width="3.6328125" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E5" s="336" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="336"/>
+      <c r="G5" s="336"/>
+      <c r="H5" s="336"/>
+      <c r="I5" s="336"/>
+      <c r="J5" s="336"/>
+      <c r="K5" s="336"/>
+    </row>
+    <row r="6" spans="3:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E6" s="346">
+        <v>0</v>
+      </c>
+      <c r="F6" s="342">
+        <v>1</v>
+      </c>
+      <c r="G6" s="342">
+        <v>2</v>
+      </c>
+      <c r="H6" s="342">
+        <v>3</v>
+      </c>
+      <c r="I6" s="342">
+        <v>4</v>
+      </c>
+      <c r="J6" s="342">
+        <v>5</v>
+      </c>
+      <c r="K6" s="342">
+        <v>6</v>
+      </c>
+      <c r="L6" s="342">
+        <v>7</v>
+      </c>
+      <c r="M6" s="343" t="s">
+        <v>164</v>
+      </c>
+      <c r="N6" s="344"/>
+      <c r="O6" s="344"/>
+      <c r="P6" s="344"/>
+      <c r="Q6" s="344"/>
+      <c r="R6" s="344"/>
+      <c r="S6" s="344"/>
+      <c r="T6" s="344"/>
+      <c r="U6" s="344"/>
+      <c r="V6" s="345"/>
+      <c r="W6" s="347"/>
+      <c r="X6" s="348"/>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C7" s="331" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="332"/>
+      <c r="E7" s="333"/>
+      <c r="F7" s="334"/>
+      <c r="G7" s="349"/>
+      <c r="H7" s="349"/>
+      <c r="I7" s="115"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="335"/>
+      <c r="L7" s="335"/>
+      <c r="M7" s="350"/>
+      <c r="N7" s="350"/>
+      <c r="O7" s="350"/>
+      <c r="P7" s="350"/>
+      <c r="Q7" s="350"/>
+      <c r="R7" s="350"/>
+      <c r="S7" s="351"/>
+      <c r="T7" s="351"/>
+      <c r="U7" s="351"/>
+      <c r="V7" s="351"/>
+      <c r="W7" s="335"/>
+      <c r="X7" s="152"/>
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C8" s="331" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="332"/>
+      <c r="E8" s="339"/>
+      <c r="F8" s="326"/>
+      <c r="G8" s="328"/>
+      <c r="H8" s="328"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="341"/>
+      <c r="T8" s="341"/>
+      <c r="U8" s="341"/>
+      <c r="V8" s="341"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="3"/>
+    </row>
+    <row r="9" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C9" s="331" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="332"/>
+      <c r="E9" s="337"/>
+      <c r="F9" s="327"/>
+      <c r="G9" s="329"/>
+      <c r="H9" s="329"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
+      <c r="V9" s="42"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="3"/>
+    </row>
+    <row r="10" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="E10" s="352"/>
+      <c r="F10" s="340"/>
+      <c r="G10" s="330"/>
+      <c r="H10" s="330"/>
+      <c r="I10" s="227"/>
+      <c r="J10" s="227"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="3"/>
+    </row>
+    <row r="11" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="E11" s="353"/>
+      <c r="F11" s="338"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="3"/>
+    </row>
+    <row r="12" spans="3:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E12" s="154"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="5"/>
+    </row>
+    <row r="13" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="E13" s="332" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="332"/>
+      <c r="G13" s="332" t="s">
+        <v>161</v>
+      </c>
+      <c r="H13" s="332"/>
+      <c r="I13" s="332" t="s">
+        <v>163</v>
+      </c>
+      <c r="J13" s="332"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="M6:V6"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -12083,7 +12519,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
+    <oddHeader>&amp;L&amp;"Arial"&amp;11&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -12271,7 +12707,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
+    <oddHeader>&amp;L&amp;"Arial"&amp;11&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -12507,7 +12943,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
+    <oddHeader>&amp;L&amp;"Arial"&amp;11&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -13796,7 +14232,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
+    <oddHeader>&amp;L&amp;"Arial"&amp;11&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -13837,21 +14273,21 @@
       <c r="J2" s="45"/>
       <c r="K2" s="45"/>
       <c r="L2" s="45"/>
-      <c r="M2" s="280" t="s">
+      <c r="M2" s="289" t="s">
         <v>144</v>
       </c>
-      <c r="N2" s="281"/>
-      <c r="O2" s="281"/>
-      <c r="P2" s="281"/>
-      <c r="Q2" s="281"/>
-      <c r="R2" s="282"/>
-      <c r="S2" s="277" t="s">
+      <c r="N2" s="290"/>
+      <c r="O2" s="290"/>
+      <c r="P2" s="290"/>
+      <c r="Q2" s="290"/>
+      <c r="R2" s="291"/>
+      <c r="S2" s="286" t="s">
         <v>143</v>
       </c>
-      <c r="T2" s="278"/>
-      <c r="U2" s="278"/>
-      <c r="V2" s="278"/>
-      <c r="W2" s="279"/>
+      <c r="T2" s="287"/>
+      <c r="U2" s="287"/>
+      <c r="V2" s="287"/>
+      <c r="W2" s="288"/>
       <c r="X2" s="45"/>
     </row>
     <row r="3" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -22976,7 +23412,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
+    <oddHeader>&amp;L&amp;"Arial"&amp;11&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>